<commit_message>
Prepared demo and example file for HYGOV.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_hygov.xlsx
+++ b/andes/cases/ieee14/ieee14_hygov.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F6D679-FFF2-1640-8F05-8D7CD92C42D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB24E0D-1716-A248-A3D7-5F9EA43C34E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36480" yWindow="1540" windowWidth="34560" windowHeight="19000" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1720" yWindow="1420" windowWidth="34560" windowHeight="19000" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E613F46-39BC-604D-A2CE-C40FAEE39A69}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1095,7 +1095,7 @@
         <v>166</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>118</v>
+        <v>172</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
@@ -5053,7 +5053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AC20" sqref="AC20"/>
     </sheetView>

</xml_diff>

<commit_message>
Fixed one equation of HYGOV4
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_hygov.xlsx
+++ b/andes/cases/ieee14/ieee14_hygov.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\zaidmahmood\repos\andes\andes\cases\ieee14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB24E0D-1716-A248-A3D7-5F9EA43C34E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81241BFA-E35C-4708-B6D3-9A2F026B0DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="1420" windowWidth="34560" windowHeight="19000" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1839" yWindow="1839" windowWidth="17426" windowHeight="8955" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -558,7 +558,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -942,9 +942,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,7 +967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -990,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1022,13 +1022,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E613F46-39BC-604D-A2CE-C40FAEE39A69}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="4" customFormat="1">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1148,9 +1148,9 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1372,9 +1372,9 @@
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1494,9 +1494,9 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1830,9 +1830,9 @@
       <selection pane="bottomLeft" activeCell="N38" sqref="N38:O38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1950,9 +1950,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2626,9 +2626,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3062,9 +3062,9 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3361,9 +3361,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3498,9 +3498,9 @@
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -4888,9 +4888,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5000,9 +5000,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5058,9 +5058,9 @@
       <selection pane="bottomLeft" activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28">
       <c r="A6" s="1">
         <v>4</v>
       </c>

</xml_diff>